<commit_message>
add estoque wms para send_fulfillment
</commit_message>
<xml_diff>
--- a/Data/Base/relacao_full_tiny.xlsx
+++ b/Data/Base/relacao_full_tiny.xlsx
@@ -10,14 +10,14 @@
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Musical!$A$1:$H$1058</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Cristiano!$A$1:$H$109</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'M A Bueno'!$A$1:$H$1012</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'M A Bueno'!$A$1:$H$1005</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6024" uniqueCount="2554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5989" uniqueCount="2553">
   <si>
     <t>inventory_id</t>
   </si>
@@ -7591,48 +7591,48 @@
     <t>MLB3699462992</t>
   </si>
   <si>
+    <t>MJBI92668</t>
+  </si>
+  <si>
+    <t>MLB4188765884</t>
+  </si>
+  <si>
+    <t>C4L44001</t>
+  </si>
+  <si>
+    <t>Bateria Infantil Luen Star Kids Reforçada Com Banco Chimbal</t>
+  </si>
+  <si>
+    <t>Bateria infantil</t>
+  </si>
+  <si>
+    <t>OHEG93627</t>
+  </si>
+  <si>
+    <t>C4L44001-1</t>
+  </si>
+  <si>
+    <t>759569737</t>
+  </si>
+  <si>
+    <t>7908334116714</t>
+  </si>
+  <si>
+    <t>GBBH94973</t>
+  </si>
+  <si>
+    <t>C4L44001-2</t>
+  </si>
+  <si>
+    <t>759569733</t>
+  </si>
+  <si>
+    <t>7908334116707</t>
+  </si>
+  <si>
     <t>ZENV95069</t>
   </si>
   <si>
-    <t>MLB4188765884</t>
-  </si>
-  <si>
-    <t>C4L44001</t>
-  </si>
-  <si>
-    <t>Bateria Infantil Luen Star Kids Reforçada Com Banco Chimbal</t>
-  </si>
-  <si>
-    <t>Bateria infantil</t>
-  </si>
-  <si>
-    <t>OHEG93627</t>
-  </si>
-  <si>
-    <t>C4L44001-1</t>
-  </si>
-  <si>
-    <t>759569737</t>
-  </si>
-  <si>
-    <t>7908334116714</t>
-  </si>
-  <si>
-    <t>MJBI92668</t>
-  </si>
-  <si>
-    <t>GBBH94973</t>
-  </si>
-  <si>
-    <t>C4L44001-2</t>
-  </si>
-  <si>
-    <t>759569733</t>
-  </si>
-  <si>
-    <t>7908334116707</t>
-  </si>
-  <si>
     <t>C4L44001-3</t>
   </si>
   <si>
@@ -7642,9 +7642,6 @@
     <t>7908334116691</t>
   </si>
   <si>
-    <t>C4L44001-4</t>
-  </si>
-  <si>
     <t>GZIL94761</t>
   </si>
   <si>
@@ -7672,13 +7669,13 @@
     <t>MLB4238572628</t>
   </si>
   <si>
+    <t>EXWA94047</t>
+  </si>
+  <si>
+    <t>BBIN94522</t>
+  </si>
+  <si>
     <t>TAEG94465</t>
-  </si>
-  <si>
-    <t>EXWA94047</t>
-  </si>
-  <si>
-    <t>BBIN94522</t>
   </si>
 </sst>
 </file>
@@ -34933,8 +34930,8 @@
     <col customWidth="1" min="4" max="4" width="59.25"/>
     <col customWidth="1" min="5" max="5" width="11.25"/>
     <col customWidth="1" min="6" max="6" width="24.13"/>
-    <col customWidth="1" min="7" max="7" width="19.0"/>
-    <col customWidth="1" min="8" max="8" width="16.13"/>
+    <col customWidth="1" min="7" max="7" width="22.0"/>
+    <col customWidth="1" min="8" max="8" width="14.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -41003,19 +41000,19 @@
         <v>2525</v>
       </c>
       <c r="C234" s="19" t="s">
-        <v>2530</v>
+        <v>2534</v>
       </c>
       <c r="D234" s="19" t="s">
         <v>2527</v>
       </c>
-      <c r="E234" s="19">
-        <v>7.59569737E8</v>
-      </c>
-      <c r="F234" s="16">
-        <v>7.908334116714E12</v>
-      </c>
-      <c r="G234" s="19">
-        <v>1.0</v>
+      <c r="E234" s="21" t="s">
+        <v>2535</v>
+      </c>
+      <c r="F234" s="22" t="s">
+        <v>2536</v>
+      </c>
+      <c r="G234" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="H234" s="19" t="s">
         <v>2528</v>
@@ -41023,22 +41020,22 @@
     </row>
     <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="19" t="s">
-        <v>2534</v>
+        <v>2537</v>
       </c>
       <c r="B235" s="19" t="s">
         <v>2525</v>
       </c>
       <c r="C235" s="19" t="s">
-        <v>2535</v>
+        <v>2538</v>
       </c>
       <c r="D235" s="19" t="s">
         <v>2527</v>
       </c>
       <c r="E235" s="21" t="s">
-        <v>2536</v>
+        <v>2539</v>
       </c>
       <c r="F235" s="22" t="s">
-        <v>2537</v>
+        <v>2540</v>
       </c>
       <c r="G235" s="21" t="s">
         <v>14</v>
@@ -41049,126 +41046,126 @@
     </row>
     <row r="236" ht="15.75" customHeight="1">
       <c r="A236" s="19" t="s">
-        <v>2533</v>
+        <v>2541</v>
       </c>
       <c r="B236" s="19" t="s">
-        <v>2525</v>
+        <v>2542</v>
       </c>
       <c r="C236" s="19" t="s">
-        <v>2535</v>
+        <v>2464</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E236" s="19">
-        <v>7.59569733E8</v>
-      </c>
-      <c r="F236" s="16">
-        <v>7.908334116707E12</v>
-      </c>
-      <c r="G236" s="19">
-        <v>1.0</v>
+        <v>2465</v>
+      </c>
+      <c r="E236" s="21" t="s">
+        <v>2466</v>
+      </c>
+      <c r="F236" s="22" t="s">
+        <v>2467</v>
+      </c>
+      <c r="G236" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="H236" s="19" t="s">
-        <v>2528</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
       <c r="A237" s="19" t="s">
-        <v>2524</v>
+        <v>2543</v>
       </c>
       <c r="B237" s="19" t="s">
-        <v>2525</v>
+        <v>2542</v>
       </c>
       <c r="C237" s="19" t="s">
-        <v>2538</v>
+        <v>2469</v>
       </c>
       <c r="D237" s="19" t="s">
-        <v>2527</v>
+        <v>2465</v>
       </c>
       <c r="E237" s="21" t="s">
-        <v>2539</v>
+        <v>2470</v>
       </c>
       <c r="F237" s="22" t="s">
-        <v>2540</v>
+        <v>2471</v>
       </c>
       <c r="G237" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H237" s="19" t="s">
-        <v>2528</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="19" t="s">
-        <v>2533</v>
+        <v>2544</v>
       </c>
       <c r="B238" s="19" t="s">
-        <v>2525</v>
+        <v>2542</v>
       </c>
       <c r="C238" s="19" t="s">
-        <v>2538</v>
+        <v>2473</v>
       </c>
       <c r="D238" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E238" s="19">
-        <v>7.59569721E8</v>
-      </c>
-      <c r="F238" s="16">
-        <v>7.908334116691E12</v>
-      </c>
-      <c r="G238" s="19">
-        <v>1.0</v>
+        <v>2465</v>
+      </c>
+      <c r="E238" s="21" t="s">
+        <v>2474</v>
+      </c>
+      <c r="F238" s="22" t="s">
+        <v>2475</v>
+      </c>
+      <c r="G238" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="H238" s="19" t="s">
-        <v>2528</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="19" t="s">
-        <v>2533</v>
+        <v>2545</v>
       </c>
       <c r="B239" s="19" t="s">
-        <v>2525</v>
+        <v>2542</v>
       </c>
       <c r="C239" s="19" t="s">
-        <v>2541</v>
+        <v>2477</v>
       </c>
       <c r="D239" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E239" s="19">
-        <v>7.59569709E8</v>
-      </c>
-      <c r="F239" s="16">
-        <v>7.908334116684E12</v>
-      </c>
-      <c r="G239" s="19">
-        <v>1.0</v>
+        <v>2465</v>
+      </c>
+      <c r="E239" s="21" t="s">
+        <v>2478</v>
+      </c>
+      <c r="F239" s="22" t="s">
+        <v>2479</v>
+      </c>
+      <c r="G239" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="H239" s="19" t="s">
-        <v>2528</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="19" t="s">
+        <v>2546</v>
+      </c>
+      <c r="B240" s="19" t="s">
         <v>2542</v>
       </c>
-      <c r="B240" s="19" t="s">
-        <v>2543</v>
-      </c>
       <c r="C240" s="19" t="s">
-        <v>2464</v>
+        <v>2481</v>
       </c>
       <c r="D240" s="19" t="s">
         <v>2465</v>
       </c>
       <c r="E240" s="21" t="s">
-        <v>2466</v>
+        <v>2482</v>
       </c>
       <c r="F240" s="22" t="s">
-        <v>2467</v>
+        <v>2483</v>
       </c>
       <c r="G240" s="21" t="s">
         <v>14</v>
@@ -41179,22 +41176,22 @@
     </row>
     <row r="241" ht="15.75" customHeight="1">
       <c r="A241" s="19" t="s">
-        <v>2544</v>
+        <v>2547</v>
       </c>
       <c r="B241" s="19" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="C241" s="19" t="s">
-        <v>2469</v>
+        <v>2485</v>
       </c>
       <c r="D241" s="19" t="s">
         <v>2465</v>
       </c>
       <c r="E241" s="21" t="s">
-        <v>2470</v>
+        <v>2486</v>
       </c>
       <c r="F241" s="22" t="s">
-        <v>2471</v>
+        <v>2487</v>
       </c>
       <c r="G241" s="21" t="s">
         <v>14</v>
@@ -41205,289 +41202,177 @@
     </row>
     <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="19" t="s">
-        <v>2545</v>
+        <v>2548</v>
       </c>
       <c r="B242" s="19" t="s">
-        <v>2543</v>
+        <v>2549</v>
       </c>
       <c r="C242" s="19" t="s">
-        <v>2473</v>
+        <v>2530</v>
       </c>
       <c r="D242" s="19" t="s">
-        <v>2465</v>
+        <v>2527</v>
       </c>
       <c r="E242" s="21" t="s">
-        <v>2474</v>
+        <v>2531</v>
       </c>
       <c r="F242" s="22" t="s">
-        <v>2475</v>
+        <v>2532</v>
       </c>
       <c r="G242" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H242" s="19" t="s">
-        <v>1172</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="19" t="s">
-        <v>2546</v>
+        <v>2550</v>
       </c>
       <c r="B243" s="19" t="s">
-        <v>2543</v>
+        <v>2549</v>
       </c>
       <c r="C243" s="19" t="s">
-        <v>2477</v>
+        <v>2534</v>
       </c>
       <c r="D243" s="19" t="s">
-        <v>2465</v>
+        <v>2527</v>
       </c>
       <c r="E243" s="21" t="s">
-        <v>2478</v>
+        <v>2535</v>
       </c>
       <c r="F243" s="22" t="s">
-        <v>2479</v>
+        <v>2536</v>
       </c>
       <c r="G243" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H243" s="19" t="s">
-        <v>1172</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="19" t="s">
-        <v>2547</v>
+        <v>2551</v>
       </c>
       <c r="B244" s="19" t="s">
-        <v>2543</v>
+        <v>2549</v>
       </c>
       <c r="C244" s="19" t="s">
-        <v>2481</v>
+        <v>2538</v>
       </c>
       <c r="D244" s="19" t="s">
-        <v>2465</v>
+        <v>2527</v>
       </c>
       <c r="E244" s="21" t="s">
-        <v>2482</v>
+        <v>2539</v>
       </c>
       <c r="F244" s="22" t="s">
-        <v>2483</v>
+        <v>2540</v>
       </c>
       <c r="G244" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H244" s="19" t="s">
-        <v>1172</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="19" t="s">
-        <v>2548</v>
+        <v>2552</v>
       </c>
       <c r="B245" s="19" t="s">
-        <v>2543</v>
+        <v>2549</v>
       </c>
       <c r="C245" s="19" t="s">
-        <v>2485</v>
+        <v>2526</v>
       </c>
       <c r="D245" s="19" t="s">
-        <v>2465</v>
-      </c>
-      <c r="E245" s="21" t="s">
-        <v>2486</v>
-      </c>
-      <c r="F245" s="22" t="s">
-        <v>2487</v>
-      </c>
-      <c r="G245" s="21" t="s">
-        <v>14</v>
+        <v>2527</v>
+      </c>
+      <c r="E245" s="19">
+        <v>7.59569709E8</v>
+      </c>
+      <c r="F245" s="16">
+        <v>7.908334116684E12</v>
+      </c>
+      <c r="G245" s="19">
+        <v>1.0</v>
       </c>
       <c r="H245" s="19" t="s">
-        <v>1172</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="19" t="s">
-        <v>2549</v>
-      </c>
-      <c r="B246" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C246" s="19" t="s">
-        <v>2530</v>
-      </c>
-      <c r="D246" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E246" s="21" t="s">
-        <v>2531</v>
-      </c>
-      <c r="F246" s="22" t="s">
-        <v>2532</v>
-      </c>
-      <c r="G246" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H246" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A246" s="19"/>
+      <c r="B246" s="19"/>
+      <c r="C246" s="19"/>
+      <c r="D246" s="19"/>
+      <c r="E246" s="19"/>
+      <c r="F246" s="16"/>
+      <c r="G246" s="19"/>
+      <c r="H246" s="19"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="19" t="s">
-        <v>2551</v>
-      </c>
-      <c r="B247" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C247" s="19" t="s">
-        <v>2530</v>
-      </c>
-      <c r="D247" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E247" s="19">
-        <v>7.59569737E8</v>
-      </c>
-      <c r="F247" s="16">
-        <v>7.908334116714E12</v>
-      </c>
-      <c r="G247" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="H247" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A247" s="19"/>
+      <c r="B247" s="19"/>
+      <c r="C247" s="19"/>
+      <c r="D247" s="19"/>
+      <c r="E247" s="19"/>
+      <c r="F247" s="16"/>
+      <c r="G247" s="19"/>
+      <c r="H247" s="19"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="19" t="s">
-        <v>2552</v>
-      </c>
-      <c r="B248" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C248" s="19" t="s">
-        <v>2535</v>
-      </c>
-      <c r="D248" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E248" s="21" t="s">
-        <v>2536</v>
-      </c>
-      <c r="F248" s="22" t="s">
-        <v>2537</v>
-      </c>
-      <c r="G248" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H248" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A248" s="19"/>
+      <c r="B248" s="19"/>
+      <c r="C248" s="19"/>
+      <c r="D248" s="19"/>
+      <c r="E248" s="19"/>
+      <c r="F248" s="16"/>
+      <c r="G248" s="19"/>
+      <c r="H248" s="19"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="19" t="s">
-        <v>2551</v>
-      </c>
-      <c r="B249" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C249" s="19" t="s">
-        <v>2535</v>
-      </c>
-      <c r="D249" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E249" s="19">
-        <v>7.59569733E8</v>
-      </c>
-      <c r="F249" s="16">
-        <v>7.908334116707E12</v>
-      </c>
-      <c r="G249" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="H249" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A249" s="19"/>
+      <c r="B249" s="19"/>
+      <c r="C249" s="19"/>
+      <c r="D249" s="19"/>
+      <c r="E249" s="19"/>
+      <c r="F249" s="16"/>
+      <c r="G249" s="19"/>
+      <c r="H249" s="19"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="19" t="s">
-        <v>2553</v>
-      </c>
-      <c r="B250" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C250" s="19" t="s">
-        <v>2538</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E250" s="21" t="s">
-        <v>2539</v>
-      </c>
-      <c r="F250" s="22" t="s">
-        <v>2540</v>
-      </c>
-      <c r="G250" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H250" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A250" s="19"/>
+      <c r="B250" s="19"/>
+      <c r="C250" s="19"/>
+      <c r="D250" s="19"/>
+      <c r="E250" s="19"/>
+      <c r="F250" s="16"/>
+      <c r="G250" s="19"/>
+      <c r="H250" s="19"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="19" t="s">
-        <v>2551</v>
-      </c>
-      <c r="B251" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C251" s="19" t="s">
-        <v>2538</v>
-      </c>
-      <c r="D251" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E251" s="19">
-        <v>7.59569721E8</v>
-      </c>
-      <c r="F251" s="16">
-        <v>7.908334116691E12</v>
-      </c>
-      <c r="G251" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="H251" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A251" s="19"/>
+      <c r="B251" s="19"/>
+      <c r="C251" s="19"/>
+      <c r="D251" s="19"/>
+      <c r="E251" s="19"/>
+      <c r="F251" s="16"/>
+      <c r="G251" s="19"/>
+      <c r="H251" s="19"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="19" t="s">
-        <v>2551</v>
-      </c>
-      <c r="B252" s="19" t="s">
-        <v>2550</v>
-      </c>
-      <c r="C252" s="19" t="s">
-        <v>2541</v>
-      </c>
-      <c r="D252" s="19" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E252" s="19">
-        <v>7.59569709E8</v>
-      </c>
-      <c r="F252" s="16">
-        <v>7.908334116684E12</v>
-      </c>
-      <c r="G252" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="H252" s="19" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A252" s="19"/>
+      <c r="B252" s="19"/>
+      <c r="C252" s="19"/>
+      <c r="D252" s="19"/>
+      <c r="E252" s="19"/>
+      <c r="F252" s="16"/>
+      <c r="G252" s="19"/>
+      <c r="H252" s="19"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
       <c r="A253" s="19"/>
@@ -43420,74 +43305,25 @@
       <c r="H445" s="19"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="A446" s="19"/>
-      <c r="B446" s="19"/>
-      <c r="C446" s="19"/>
-      <c r="D446" s="19"/>
-      <c r="E446" s="19"/>
-      <c r="F446" s="16"/>
-      <c r="G446" s="19"/>
-      <c r="H446" s="19"/>
+      <c r="F446" s="10"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="A447" s="19"/>
-      <c r="B447" s="19"/>
-      <c r="C447" s="19"/>
-      <c r="D447" s="19"/>
-      <c r="E447" s="19"/>
-      <c r="F447" s="16"/>
-      <c r="G447" s="19"/>
-      <c r="H447" s="19"/>
+      <c r="F447" s="10"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="A448" s="19"/>
-      <c r="B448" s="19"/>
-      <c r="C448" s="19"/>
-      <c r="D448" s="19"/>
-      <c r="E448" s="19"/>
-      <c r="F448" s="16"/>
-      <c r="G448" s="19"/>
-      <c r="H448" s="19"/>
+      <c r="F448" s="10"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="A449" s="19"/>
-      <c r="B449" s="19"/>
-      <c r="C449" s="19"/>
-      <c r="D449" s="19"/>
-      <c r="E449" s="19"/>
-      <c r="F449" s="16"/>
-      <c r="G449" s="19"/>
-      <c r="H449" s="19"/>
+      <c r="F449" s="10"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="A450" s="19"/>
-      <c r="B450" s="19"/>
-      <c r="C450" s="19"/>
-      <c r="D450" s="19"/>
-      <c r="E450" s="19"/>
-      <c r="F450" s="16"/>
-      <c r="G450" s="19"/>
-      <c r="H450" s="19"/>
+      <c r="F450" s="10"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="A451" s="19"/>
-      <c r="B451" s="19"/>
-      <c r="C451" s="19"/>
-      <c r="D451" s="19"/>
-      <c r="E451" s="19"/>
-      <c r="F451" s="16"/>
-      <c r="G451" s="19"/>
-      <c r="H451" s="19"/>
+      <c r="F451" s="10"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="A452" s="19"/>
-      <c r="B452" s="19"/>
-      <c r="C452" s="19"/>
-      <c r="D452" s="19"/>
-      <c r="E452" s="19"/>
-      <c r="F452" s="16"/>
-      <c r="G452" s="19"/>
-      <c r="H452" s="19"/>
+      <c r="F452" s="10"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
       <c r="F453" s="10"/>
@@ -45148,31 +44984,10 @@
     <row r="1005" ht="15.75" customHeight="1">
       <c r="F1005" s="10"/>
     </row>
-    <row r="1006" ht="15.75" customHeight="1">
-      <c r="F1006" s="10"/>
-    </row>
-    <row r="1007" ht="15.75" customHeight="1">
-      <c r="F1007" s="10"/>
-    </row>
-    <row r="1008" ht="15.75" customHeight="1">
-      <c r="F1008" s="10"/>
-    </row>
-    <row r="1009" ht="15.75" customHeight="1">
-      <c r="F1009" s="10"/>
-    </row>
-    <row r="1010" ht="15.75" customHeight="1">
-      <c r="F1010" s="10"/>
-    </row>
-    <row r="1011" ht="15.75" customHeight="1">
-      <c r="F1011" s="10"/>
-    </row>
-    <row r="1012" ht="15.75" customHeight="1">
-      <c r="F1012" s="10"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$1012">
-    <sortState ref="A1:H1012">
-      <sortCondition ref="B1:B1012"/>
+  <autoFilter ref="$A$1:$H$1005">
+    <sortState ref="A1:H1005">
+      <sortCondition ref="B1:B1005"/>
     </sortState>
   </autoFilter>
   <printOptions/>

</xml_diff>